<commit_message>
Update Leave Card 12/22/2023 10:59 AM
</commit_message>
<xml_diff>
--- a/BAROA, JONA ANGCAYA.xlsx
+++ b/BAROA, JONA ANGCAYA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5B8FFD-9560-4EC6-BD99-049C997A8865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE69673-F405-4187-9D6C-96F4A58F10B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="48" windowWidth="23016" windowHeight="12312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>PERIOD</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>4/3-5,10-14/2023</t>
+  </si>
+  <si>
+    <t>10/23,24/2023</t>
   </si>
 </sst>
 </file>
@@ -2673,7 +2676,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3696" topLeftCell="A55" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="B65:C65"/>
+      <selection pane="bottomLeft" activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2834,7 +2837,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>24.75</v>
+        <v>27.75</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2844,7 +2847,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>51.75</v>
+        <v>56.75</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -3993,13 +3996,15 @@
       <c r="B64" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C64" s="13"/>
+      <c r="C64" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D64" s="39"/>
       <c r="E64" s="9"/>
       <c r="F64" s="20"/>
-      <c r="G64" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G64" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H64" s="39">
         <v>1</v>
@@ -4015,13 +4020,15 @@
         <v>45138</v>
       </c>
       <c r="B65" s="20"/>
-      <c r="C65" s="13"/>
+      <c r="C65" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D65" s="39"/>
       <c r="E65" s="9"/>
       <c r="F65" s="20"/>
-      <c r="G65" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G65" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H65" s="39"/>
       <c r="I65" s="9"/>
@@ -4033,13 +4040,15 @@
         <v>45169</v>
       </c>
       <c r="B66" s="20"/>
-      <c r="C66" s="13"/>
+      <c r="C66" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D66" s="39"/>
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G66" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H66" s="39"/>
       <c r="I66" s="9"/>
@@ -4051,13 +4060,15 @@
         <v>45199</v>
       </c>
       <c r="B67" s="20"/>
-      <c r="C67" s="13"/>
+      <c r="C67" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D67" s="39"/>
       <c r="E67" s="9"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G67" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H67" s="39"/>
       <c r="I67" s="9"/>
@@ -4068,9 +4079,13 @@
       <c r="A68" s="40">
         <v>45230</v>
       </c>
-      <c r="B68" s="20"/>
+      <c r="B68" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C68" s="13"/>
-      <c r="D68" s="39"/>
+      <c r="D68" s="39">
+        <v>2</v>
+      </c>
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
       <c r="G68" s="13" t="str">
@@ -4080,7 +4095,9 @@
       <c r="H68" s="39"/>
       <c r="I68" s="9"/>
       <c r="J68" s="11"/>
-      <c r="K68" s="20"/>
+      <c r="K68" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">

</xml_diff>